<commit_message>
commiting the test cases
</commit_message>
<xml_diff>
--- a/TestCases/Testcases.xlsx
+++ b/TestCases/Testcases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811C631D-4431-4CF6-BBDA-838D81C15B39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E6023B-C575-4A27-9E30-11895B6FFEBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1050,7 +1050,7 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C77"/>
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1244,7 +1244,7 @@
         <v>24</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D19" s="22" t="s">
         <v>6</v>
@@ -1258,7 +1258,7 @@
         <v>64</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>6</v>
@@ -1272,7 +1272,7 @@
         <v>25</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>6</v>
@@ -1286,7 +1286,7 @@
         <v>26</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>6</v>
@@ -1300,7 +1300,7 @@
         <v>36</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>6</v>
@@ -1314,7 +1314,7 @@
         <v>41</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>6</v>
@@ -1328,7 +1328,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>6</v>
@@ -1342,7 +1342,7 @@
         <v>45</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>6</v>
@@ -1356,7 +1356,7 @@
         <v>73</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>6</v>
@@ -1370,7 +1370,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>6</v>
@@ -1384,7 +1384,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>6</v>
@@ -1398,7 +1398,7 @@
         <v>37</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>6</v>
@@ -1412,7 +1412,7 @@
         <v>148</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>6</v>
@@ -1426,7 +1426,7 @@
         <v>43</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>6</v>
@@ -1440,7 +1440,7 @@
         <v>55</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D33" s="22" t="s">
         <v>6</v>
@@ -1454,7 +1454,7 @@
         <v>57</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D34" s="22" t="s">
         <v>6</v>
@@ -1468,7 +1468,7 @@
         <v>48</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D35" s="22" t="s">
         <v>6</v>
@@ -1482,7 +1482,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>6</v>
@@ -1496,7 +1496,7 @@
         <v>63</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D37" s="22" t="s">
         <v>6</v>
@@ -1510,7 +1510,7 @@
         <v>53</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>6</v>
@@ -1524,7 +1524,7 @@
         <v>46</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>6</v>
@@ -1538,7 +1538,7 @@
         <v>74</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>6</v>
@@ -1552,7 +1552,7 @@
         <v>65</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>6</v>
@@ -1566,7 +1566,7 @@
         <v>66</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>6</v>
@@ -1580,7 +1580,7 @@
         <v>67</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D43" s="22" t="s">
         <v>6</v>
@@ -1594,7 +1594,7 @@
         <v>68</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>6</v>
@@ -1608,7 +1608,7 @@
         <v>69</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>6</v>
@@ -1622,7 +1622,7 @@
         <v>70</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D46" s="22" t="s">
         <v>6</v>
@@ -1636,7 +1636,7 @@
         <v>71</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>6</v>
@@ -1650,7 +1650,7 @@
         <v>88</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D48" s="16" t="s">
         <v>6</v>
@@ -1664,7 +1664,7 @@
         <v>89</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D49" s="16" t="s">
         <v>6</v>
@@ -1678,7 +1678,7 @@
         <v>90</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D50" s="16" t="s">
         <v>6</v>
@@ -1692,7 +1692,7 @@
         <v>91</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D51" s="16" t="s">
         <v>6</v>
@@ -1706,7 +1706,7 @@
         <v>92</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D52" s="16" t="s">
         <v>6</v>
@@ -1720,7 +1720,7 @@
         <v>93</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D53" s="16" t="s">
         <v>6</v>
@@ -1734,7 +1734,7 @@
         <v>94</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D54" s="16" t="s">
         <v>6</v>
@@ -1748,7 +1748,7 @@
         <v>95</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D55" s="16" t="s">
         <v>6</v>
@@ -1762,7 +1762,7 @@
         <v>96</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D56" s="16" t="s">
         <v>6</v>
@@ -1776,7 +1776,7 @@
         <v>97</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D57" s="16" t="s">
         <v>6</v>
@@ -1790,7 +1790,7 @@
         <v>98</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D58" s="16" t="s">
         <v>6</v>
@@ -1804,7 +1804,7 @@
         <v>99</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D59" s="16" t="s">
         <v>6</v>
@@ -1818,7 +1818,7 @@
         <v>100</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D60" s="16" t="s">
         <v>6</v>
@@ -1832,7 +1832,7 @@
         <v>101</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D61" s="16" t="s">
         <v>6</v>
@@ -1846,7 +1846,7 @@
         <v>103</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D62" s="16" t="s">
         <v>6</v>
@@ -1860,7 +1860,7 @@
         <v>105</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D63" s="16" t="s">
         <v>6</v>
@@ -1874,7 +1874,7 @@
         <v>106</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D64" s="16" t="s">
         <v>6</v>
@@ -1888,7 +1888,7 @@
         <v>107</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D65" s="16" t="s">
         <v>6</v>
@@ -1902,7 +1902,7 @@
         <v>108</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D66" s="16" t="s">
         <v>6</v>
@@ -1916,7 +1916,7 @@
         <v>110</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D67" s="16" t="s">
         <v>6</v>
@@ -1930,7 +1930,7 @@
         <v>111</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D68" s="16" t="s">
         <v>6</v>
@@ -1944,7 +1944,7 @@
         <v>112</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D69" s="16" t="s">
         <v>6</v>
@@ -1958,7 +1958,7 @@
         <v>114</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D70" s="16" t="s">
         <v>6</v>
@@ -1972,7 +1972,7 @@
         <v>116</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D71" s="16" t="s">
         <v>6</v>
@@ -1986,7 +1986,7 @@
         <v>118</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D72" s="16" t="s">
         <v>6</v>
@@ -2000,7 +2000,7 @@
         <v>120</v>
       </c>
       <c r="C73" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D73" s="16" t="s">
         <v>6</v>
@@ -2014,7 +2014,7 @@
         <v>122</v>
       </c>
       <c r="C74" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D74" s="16" t="s">
         <v>6</v>
@@ -2028,7 +2028,7 @@
         <v>124</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D75" s="16" t="s">
         <v>6</v>
@@ -2042,7 +2042,7 @@
         <v>115</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D76" s="16" t="s">
         <v>6</v>
@@ -2056,7 +2056,7 @@
         <v>113</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D77" s="16" t="s">
         <v>6</v>
@@ -2090,13 +2090,13 @@
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:C14 C16:C27 C28:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:C14 C16:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Regression,Defect Verification,Functional"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D28:D29 D18:D22 D78 D48:D77" xr:uid="{EAB48051-5C6D-4B58-B007-F9A526BDCDA0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D28:D29 D18:D22 D48:D78" xr:uid="{EAB48051-5C6D-4B58-B007-F9A526BDCDA0}">
       <formula1>"P,N"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>